<commit_message>
ajout mapping global page d'accueil 1a8d26fe4cd173eeccfeb8dad14d7515bd6b92c9
</commit_message>
<xml_diff>
--- a/update-mapping-pn13/ig/StructureDefinition-oncofair-medicationrequest-element.xlsx
+++ b/update-mapping-pn13/ig/StructureDefinition-oncofair-medicationrequest-element.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-17T15:02:03+00:00</t>
+    <t>2024-06-17T15:41:32+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -12765,10 +12765,10 @@
         <v>104</v>
       </c>
       <c r="AK73" t="s" s="2">
-        <v>80</v>
+        <v>527</v>
       </c>
       <c r="AL73" t="s" s="2">
-        <v>527</v>
+        <v>80</v>
       </c>
       <c r="AM73" t="s" s="2">
         <v>521</v>
@@ -13497,10 +13497,10 @@
         <v>104</v>
       </c>
       <c r="AK79" t="s" s="2">
-        <v>80</v>
+        <v>554</v>
       </c>
       <c r="AL79" t="s" s="2">
-        <v>554</v>
+        <v>80</v>
       </c>
       <c r="AM79" t="s" s="2">
         <v>521</v>
@@ -14229,10 +14229,10 @@
         <v>104</v>
       </c>
       <c r="AK85" t="s" s="2">
-        <v>80</v>
+        <v>564</v>
       </c>
       <c r="AL85" t="s" s="2">
-        <v>564</v>
+        <v>80</v>
       </c>
       <c r="AM85" t="s" s="2">
         <v>521</v>
@@ -15449,10 +15449,10 @@
         <v>104</v>
       </c>
       <c r="AK95" t="s" s="2">
-        <v>80</v>
+        <v>587</v>
       </c>
       <c r="AL95" t="s" s="2">
-        <v>587</v>
+        <v>80</v>
       </c>
       <c r="AM95" t="s" s="2">
         <v>80</v>
@@ -15574,10 +15574,10 @@
         <v>104</v>
       </c>
       <c r="AK96" t="s" s="2">
-        <v>80</v>
+        <v>596</v>
       </c>
       <c r="AL96" t="s" s="2">
-        <v>596</v>
+        <v>80</v>
       </c>
       <c r="AM96" t="s" s="2">
         <v>80</v>

</xml_diff>